<commit_message>
Fix error in printing in POD and Fix not showing color coding in PR summary
</commit_message>
<xml_diff>
--- a/PR Summary.xlsx
+++ b/PR Summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>PR Summary 2021</t>
   </si>
@@ -92,70 +92,32 @@
     <t>End User's Comments</t>
   </si>
   <si>
-    <t>2021-06-10</t>
-  </si>
-  <si>
-    <t>bacolod</t>
-  </si>
-  <si>
-    <t>Lorem Ipsum 233323</t>
-  </si>
-  <si>
-    <t>Lorem Ipsum 233223</t>
-  </si>
-  <si>
-    <t>ITB21-1000-CNPR</t>
-  </si>
-  <si>
-    <t>jush</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orig.: 10.00 pc/s
-Rev. 1: 5.00 pc/s
-Rev. 2: 8.00 pc/s
+    <t>2021-11-23</t>
+  </si>
+  <si>
+    <t>BCD</t>
+  </si>
+  <si>
+    <t>Replacement of damage UPS</t>
+  </si>
+  <si>
+    <t>Bacolod HR Admin</t>
+  </si>
+  <si>
+    <t>HRB21-1000-CNPR</t>
+  </si>
+  <si>
+    <t>Syndey Sinoro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 </t>
   </si>
   <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 12234 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">06.11.2021 - Delivered DR# 1003-CNPR (2.00 pc/s)
-</t>
-  </si>
-  <si>
-    <t>Partially Delivered</t>
-  </si>
-  <si>
-    <t>Jun 11, 2021</t>
-  </si>
-  <si>
-    <t>✓</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 15234 </t>
-  </si>
-  <si>
-    <t>For RFQ 
--On Hold Date: 2021-06-10 04:25:14
- -On Hold By: Jonah Benares</t>
-  </si>
-  <si>
-    <t>On-Hold</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 29123 </t>
+    <t xml:space="preserve">Adapter </t>
   </si>
   <si>
     <t xml:space="preserve">For RFQ 
@@ -163,6 +125,92 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Nov 29, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Cord </t>
+  </si>
+  <si>
+    <t>roll/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrical Tape </t>
+  </si>
+  <si>
+    <t>unit/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPS </t>
+  </si>
+  <si>
+    <t>For RFQ 
+-Recom By: Jonah Benares
+ -Recom Date: Nov 22, 2021 To Nov 27, 2021</t>
+  </si>
+  <si>
+    <t>For Recom</t>
+  </si>
+  <si>
+    <t>Additional SSD for laggy laptop</t>
+  </si>
+  <si>
+    <t>Hennelen Tanan</t>
+  </si>
+  <si>
+    <t>ITB21-1001-CNPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD 500GB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivered by CENPRI-MNL';
+                                      = 'For RFQ 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ -2021-11-23
+ -Access Frontier Technologies, Inc.
+ -2500.0000
+ -1</t>
+  </si>
+  <si>
+    <t>Replacement for damaged AVR</t>
+  </si>
+  <si>
+    <t>Bacolod Employees</t>
+  </si>
+  <si>
+    <t>ITB21-1002-CNPR</t>
+  </si>
+  <si>
+    <t>Jason Flor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVR </t>
+  </si>
+  <si>
+    <t>Repair broken internet lines</t>
+  </si>
+  <si>
+    <t>HRB21-1003-CNPR</t>
+  </si>
+  <si>
+    <t>box/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTP Cable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RJ 45 Connector Plug </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crimping Tool </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duct Tape </t>
   </si>
 </sst>
 </file>
@@ -211,13 +259,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf7ffb9"/>
+        <fgColor rgb="FFfd9c77"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFd2deff"/>
+        <fgColor rgb="FFeeccff"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -255,6 +303,18 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -277,18 +337,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -590,10 +638,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="W7" sqref="W7"/>
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -602,23 +650,23 @@
     <col min="2" max="2" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="25.85083" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="37.705078" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="21.137695" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="21.137695" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="25.85083" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="57.700195" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="23.422852" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="50.559082" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="58.842773" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="43.560791" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="23.422852" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -733,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5" s="6">
         <v>10</v>
@@ -744,138 +792,519 @@
       <c r="M5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="T5" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="6">
         <v>0</v>
       </c>
-      <c r="J6" s="9">
-        <v>2</v>
-      </c>
-      <c r="K6" s="10">
-        <v>15</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="8" t="s">
+      <c r="J6" s="5">
+        <v>3</v>
+      </c>
+      <c r="K6" s="6">
+        <v>10</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="S6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="T6" s="8" t="s">
+      <c r="N6" s="4"/>
+      <c r="O6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="6">
         <v>0</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="5">
+        <v>4</v>
+      </c>
+      <c r="K7" s="6">
+        <v>2</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <v>1</v>
+      </c>
+      <c r="K8" s="10">
+        <v>10</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="8"/>
+      <c r="O8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="14">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
+        <v>1</v>
+      </c>
+      <c r="K9" s="14">
+        <v>1</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="12"/>
+      <c r="O9" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="U9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6">
+        <v>20</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <v>2</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>2</v>
+      </c>
+      <c r="K12" s="6">
+        <v>100</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
         <v>3</v>
       </c>
-      <c r="K7" s="14">
-        <v>20</v>
-      </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="12" t="s">
+      <c r="K13" s="6">
+        <v>1</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="O7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="S7" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="T7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>4</v>
+      </c>
+      <c r="K14" s="6">
+        <v>10</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Fix report displaying of status
</commit_message>
<xml_diff>
--- a/PR Summary.xlsx
+++ b/PR Summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>PR Summary 2021</t>
   </si>
@@ -92,125 +92,107 @@
     <t>End User's Comments</t>
   </si>
   <si>
-    <t>2021-11-23</t>
-  </si>
-  <si>
-    <t>BCD</t>
-  </si>
-  <si>
-    <t>Replacement of damage UPS</t>
-  </si>
-  <si>
-    <t>Bacolod HR Admin</t>
-  </si>
-  <si>
-    <t>HRB21-1000-CNPR</t>
-  </si>
-  <si>
-    <t>Syndey Sinoro</t>
+    <t>2021-08-27</t>
+  </si>
+  <si>
+    <t>Installation of Jacket Water Injector Cooling By-Pass Line</t>
+  </si>
+  <si>
+    <t>DG Unit 4 and Unit 5</t>
+  </si>
+  <si>
+    <t>MAI21-1877-CNPR</t>
+  </si>
+  <si>
+    <t>Ruel Beato</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adapter </t>
-  </si>
-  <si>
-    <t xml:space="preserve">For RFQ 
+    <t>length</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI Pipe, Sched 40, 1 1/2" NPS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.09.2021 - Delivered DR# 3500-CNPR
 </t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>Nov 29, 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Cord </t>
-  </si>
-  <si>
-    <t>roll/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electrical Tape </t>
-  </si>
-  <si>
-    <t>unit/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPS </t>
-  </si>
-  <si>
-    <t>For RFQ 
--Recom By: Jonah Benares
- -Recom Date: Nov 22, 2021 To Nov 27, 2021</t>
-  </si>
-  <si>
-    <t>For Recom</t>
-  </si>
-  <si>
-    <t>Additional SSD for laggy laptop</t>
-  </si>
-  <si>
-    <t>Hennelen Tanan</t>
-  </si>
-  <si>
-    <t>ITB21-1001-CNPR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD 500GB </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivered by CENPRI-MNL';
-                                      = 'For RFQ 
+    <t>Fully Delivered</t>
+  </si>
+  <si>
+    <t>Sep 11, 2021</t>
+  </si>
+  <si>
+    <t>MAI-266-2021</t>
+  </si>
+  <si>
+    <t>lengths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI Pipe, Sched 40, 1" NPS </t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gate Valve, 150 lbs rating, Rising Stem, Flange Type, Cast Steel, 1 1/2" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.13.2021 - Delivered DR# 3921-CNPR
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
- -2021-11-23
- -Access Frontier Technologies, Inc.
- -2500.0000
- -1</t>
-  </si>
-  <si>
-    <t>Replacement for damaged AVR</t>
-  </si>
-  <si>
-    <t>Bacolod Employees</t>
-  </si>
-  <si>
-    <t>ITB21-1002-CNPR</t>
-  </si>
-  <si>
-    <t>Jason Flor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVR </t>
-  </si>
-  <si>
-    <t>Repair broken internet lines</t>
-  </si>
-  <si>
-    <t>HRB21-1003-CNPR</t>
-  </si>
-  <si>
-    <t>box/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UTP Cable </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RJ 45 Connector Plug </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crimping Tool </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duct Tape </t>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gate Valve, 150 lbs rating, Rising Stem, Flange Type, Cast Steel, 1" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.I. Elbow, Long Radius, Seamless, Buttweld End, Schedule 40, 1 1/2" x 90° </t>
+  </si>
+  <si>
+    <t>PO Issued</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.I. Elbow, Long Radius, Seamless, Buttweld End, Schedule 40, 1" x 90° </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slip-on Flange, Class 150, ANSI B16.5, Raised Faced, 1 1/2" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slip-on Flange, Class 150, ANSI B16.5, Raised Faced, 1" </t>
+  </si>
+  <si>
+    <t>sets</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex Head Bolt, High Tensile, Full-thread, Grade 5, M14 x 45 mm x 1.5 Pitch, with Nut &amp; Lock Washer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.04.2021 - Delivered DR# 3531-CNPR
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex Head Bolt, High Tensile, Full-thread, Grade 5, M12 x 45 mm x 1.5 Pitch, with Nut &amp; Lock Washer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">U-bolt, 1/4" x 1 1/2" NPS, w/ Nut &amp; Lock Washer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">U-bolt, 3/8" x 1" NPS, w/ Nut &amp; Lock Washer </t>
   </si>
 </sst>
 </file>
@@ -259,13 +241,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFfd9c77"/>
+        <fgColor rgb="FFbcffc7"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFeeccff"/>
+        <fgColor rgb="FFffecd0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -290,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -302,18 +284,6 @@
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -638,10 +608,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="W14" sqref="W14"/>
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -650,23 +620,23 @@
     <col min="2" max="2" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="25.85083" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="37.705078" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="69.554443" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="117.828369" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="50.559082" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="58.842773" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="43.560791" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="43.560791" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="15.281982" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="23.422852" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -762,37 +732,37 @@
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="6">
+        <v>2</v>
+      </c>
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>2</v>
-      </c>
-      <c r="K5" s="6">
-        <v>10</v>
-      </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="4"/>
       <c r="O5" s="7" t="s">
         <v>33</v>
       </c>
@@ -807,7 +777,9 @@
       <c r="T5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U5" s="5"/>
+      <c r="U5" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
     </row>
@@ -817,39 +789,39 @@
       <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
       </c>
       <c r="J6" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" s="6">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="4"/>
       <c r="O6" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="6"/>
@@ -862,7 +834,9 @@
       <c r="T6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="5"/>
+      <c r="U6" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
     </row>
@@ -872,44 +846,44 @@
       <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
       </c>
       <c r="J7" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K7" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="O7" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="S7" s="5" t="s">
         <v>35</v>
@@ -917,119 +891,123 @@
       <c r="T7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U7" s="5"/>
+      <c r="U7" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>4</v>
+      </c>
+      <c r="K8" s="6">
+        <v>3</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="10">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9">
-        <v>1</v>
-      </c>
-      <c r="K8" s="10">
-        <v>10</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="11" t="s">
+      <c r="M8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="S8" s="9" t="s">
+      <c r="O8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T8" s="8" t="s">
+      <c r="S8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
+      <c r="U8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>5</v>
+      </c>
+      <c r="K9" s="10">
+        <v>3</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="12" t="s">
+      <c r="N9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="14">
-        <v>0</v>
-      </c>
-      <c r="J9" s="13">
-        <v>1</v>
-      </c>
-      <c r="K9" s="14">
-        <v>1</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="15" t="s">
+      <c r="P9" s="8"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="T9" s="12" t="s">
+      <c r="T9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="U9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
+      <c r="U9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="4"/>
@@ -1037,44 +1015,44 @@
       <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="I10" s="6">
         <v>0</v>
       </c>
       <c r="J10" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K10" s="6">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="O10" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>35</v>
@@ -1082,7 +1060,9 @@
       <c r="T10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U10" s="5"/>
+      <c r="U10" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
     </row>
@@ -1092,44 +1072,44 @@
       <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" s="6">
         <v>0</v>
       </c>
       <c r="J11" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K11" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="O11" s="7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="S11" s="5" t="s">
         <v>35</v>
@@ -1137,7 +1117,9 @@
       <c r="T11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U11" s="5"/>
+      <c r="U11" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
     </row>
@@ -1147,44 +1129,44 @@
       <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" s="6">
         <v>0</v>
       </c>
       <c r="J12" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K12" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N12" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="O12" s="7" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="S12" s="5" t="s">
         <v>35</v>
@@ -1192,7 +1174,9 @@
       <c r="T12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U12" s="5"/>
+      <c r="U12" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
     </row>
@@ -1202,44 +1186,44 @@
       <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" s="6">
         <v>0</v>
       </c>
       <c r="J13" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K13" s="6">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="O13" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="5" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="S13" s="5" t="s">
         <v>35</v>
@@ -1247,7 +1231,9 @@
       <c r="T13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U13" s="5"/>
+      <c r="U13" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
     </row>
@@ -1257,44 +1243,44 @@
       <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I14" s="6">
         <v>0</v>
       </c>
       <c r="J14" s="5">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K14" s="6">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N14" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="O14" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="5" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="S14" s="5" t="s">
         <v>35</v>
@@ -1302,9 +1288,125 @@
       <c r="T14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U14" s="5"/>
+      <c r="U14" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>11</v>
+      </c>
+      <c r="K15" s="6">
+        <v>4</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>12</v>
+      </c>
+      <c r="K16" s="6">
+        <v>10</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
add from and to in filter of pr report
</commit_message>
<xml_diff>
--- a/PR Summary.xlsx
+++ b/PR Summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>PR Summary 2021</t>
   </si>
@@ -92,22 +92,22 @@
     <t>End User's Comments</t>
   </si>
   <si>
-    <t>2021-11-23</t>
-  </si>
-  <si>
-    <t>BCD</t>
-  </si>
-  <si>
-    <t>Replacement of damage UPS</t>
-  </si>
-  <si>
-    <t>Bacolod HR Admin</t>
-  </si>
-  <si>
-    <t>HRB21-1000-CNPR</t>
-  </si>
-  <si>
-    <t>Syndey Sinoro</t>
+    <t>2021-04-01</t>
+  </si>
+  <si>
+    <t>cons</t>
+  </si>
+  <si>
+    <t>Monitor Table and Shelves for ASPA Purpose</t>
+  </si>
+  <si>
+    <t>Monitor Table and Shelves for ASPA Enduse</t>
+  </si>
+  <si>
+    <t>ITB21-1553-CNPR</t>
+  </si>
+  <si>
+    <t>Henne</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -117,100 +117,114 @@
     <t>pc/s</t>
   </si>
   <si>
-    <t xml:space="preserve">Adapter </t>
-  </si>
-  <si>
-    <t xml:space="preserve">For RFQ 
+    <t>I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03.03.2021 - Delivered DR# 2444-CNPR
 </t>
   </si>
   <si>
+    <t>Fully Delivered</t>
+  </si>
+  <si>
+    <t>May 10, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyboard </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01.01.70</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>May 11, 2021</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitor </t>
+  </si>
+  <si>
+    <t>Canvassing Ongoing  
+-On Hold Date: 2021-03-03 03:42:36
+ -On Hold By: Jonah Benares</t>
+  </si>
+  <si>
+    <t>On-Hold</t>
+  </si>
+  <si>
+    <t>May 12, 2021</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU </t>
+  </si>
+  <si>
+    <t>cancel 03.03.21</t>
+  </si>
+  <si>
+    <t>May 13, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canvassing Ongoing 
+</t>
+  </si>
+  <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>Nov 29, 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Cord </t>
-  </si>
-  <si>
-    <t>roll/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electrical Tape </t>
-  </si>
-  <si>
-    <t>unit/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPS </t>
-  </si>
-  <si>
-    <t>For RFQ 
--Recom By: Jonah Benares
- -Recom Date: Nov 22, 2021 To Nov 27, 2021</t>
-  </si>
-  <si>
-    <t>For Recom</t>
-  </si>
-  <si>
-    <t>Additional SSD for laggy laptop</t>
-  </si>
-  <si>
-    <t>Hennelen Tanan</t>
-  </si>
-  <si>
-    <t>ITB21-1001-CNPR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD 500GB </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivered by CENPRI-MNL';
-                                      = 'For RFQ 
-</t>
+    <t>May 14, 2021</t>
   </si>
   <si>
     <t xml:space="preserve">
- -2021-11-23
- -Access Frontier Technologies, Inc.
- -2500.0000
- -1</t>
-  </si>
-  <si>
-    <t>Replacement for damaged AVR</t>
-  </si>
-  <si>
-    <t>Bacolod Employees</t>
-  </si>
-  <si>
-    <t>ITB21-1002-CNPR</t>
-  </si>
-  <si>
-    <t>Jason Flor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVR </t>
-  </si>
-  <si>
-    <t>Repair broken internet lines</t>
-  </si>
-  <si>
-    <t>HRB21-1003-CNPR</t>
-  </si>
-  <si>
-    <t>box/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UTP Cable </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RJ 45 Connector Plug </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crimping Tool </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duct Tape </t>
+ -2021-03-11
+ -A &amp; M Medcare Products Distributors
+ -575.00
+ -3</t>
+  </si>
+  <si>
+    <t>2021-03-09</t>
+  </si>
+  <si>
+    <t>Bacolod</t>
+  </si>
+  <si>
+    <t>IT Sample</t>
+  </si>
+  <si>
+    <t>ITB21-1556-CNPR</t>
+  </si>
+  <si>
+    <t>Jonah Benares</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>2021-11-23</t>
+  </si>
+  <si>
+    <t>Mar 9, 2021</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -218,7 +232,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -246,8 +260,17 @@
       <color rgb="FF000000"/>
       <name val="Arial Black"/>
     </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFff0000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,13 +282,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFfd9c77"/>
+        <fgColor rgb="FFbcffc7"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFeeccff"/>
+        <fgColor rgb="FFcacaca"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFd2deff"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -290,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -303,6 +332,45 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="4" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -313,30 +381,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -638,10 +682,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="W14" sqref="W14"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -650,23 +694,23 @@
     <col min="2" max="2" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="25.85083" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="37.705078" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="50.559082" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="49.416504" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="5.855713" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="19.995117" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="50.559082" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="58.842773" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="43.560791" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="43.560791" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="44.703369" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="23.422852" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -781,10 +825,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6">
         <v>2</v>
-      </c>
-      <c r="K5" s="6">
-        <v>10</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>31</v>
@@ -792,134 +836,142 @@
       <c r="M5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="4"/>
+      <c r="N5" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="O5" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="10">
         <v>0</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="9">
+        <v>2</v>
+      </c>
+      <c r="K6" s="10">
         <v>3</v>
       </c>
-      <c r="K6" s="6">
-        <v>10</v>
-      </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
+      <c r="N6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="15">
         <v>0</v>
       </c>
-      <c r="J7" s="5">
-        <v>4</v>
-      </c>
-      <c r="K7" s="6">
-        <v>2</v>
-      </c>
-      <c r="L7" s="6" t="s">
+      <c r="J7" s="14">
+        <v>3</v>
+      </c>
+      <c r="K7" s="15">
+        <v>1</v>
+      </c>
+      <c r="L7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
+      <c r="M7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="T7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="8"/>
@@ -946,365 +998,271 @@
         <v>0</v>
       </c>
       <c r="J8" s="9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K8" s="10">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>31</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="11" t="s">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="9" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="S8" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="U8" s="9"/>
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="14">
+      <c r="E9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="19">
         <v>0</v>
       </c>
-      <c r="J9" s="13">
-        <v>1</v>
-      </c>
-      <c r="K9" s="14">
-        <v>1</v>
-      </c>
-      <c r="L9" s="14" t="s">
+      <c r="J9" s="18">
+        <v>5</v>
+      </c>
+      <c r="K9" s="19">
+        <v>3</v>
+      </c>
+      <c r="L9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13" t="s">
+      <c r="M9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="T9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
+      <c r="O9" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="S9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="T9" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="U9" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="19">
+        <v>0</v>
+      </c>
+      <c r="J10" s="18">
+        <v>1</v>
+      </c>
+      <c r="K10" s="19">
+        <v>15</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q10" s="19">
+        <v>300</v>
+      </c>
+      <c r="R10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
-        <v>1</v>
-      </c>
-      <c r="K10" s="6">
-        <v>20</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="7" t="s">
+      <c r="S10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
+      <c r="T10" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="6">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="19">
         <v>0</v>
       </c>
-      <c r="J11" s="5">
-        <v>1</v>
-      </c>
-      <c r="K11" s="6">
+      <c r="J11" s="18">
         <v>2</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="K11" s="19">
+        <v>5</v>
+      </c>
+      <c r="L11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="5" t="s">
+      <c r="M11" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="S11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="S11" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="T11" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="6">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="19">
         <v>0</v>
       </c>
-      <c r="J12" s="5">
-        <v>2</v>
-      </c>
-      <c r="K12" s="6">
-        <v>100</v>
-      </c>
-      <c r="L12" s="6" t="s">
+      <c r="J12" s="18">
+        <v>3</v>
+      </c>
+      <c r="K12" s="19">
+        <v>10</v>
+      </c>
+      <c r="L12" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5">
-        <v>3</v>
-      </c>
-      <c r="K13" s="6">
-        <v>1</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-    </row>
-    <row r="14" spans="1:23">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>4</v>
-      </c>
-      <c r="K14" s="6">
-        <v>10</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
+      <c r="M12" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="O12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="S12" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="T12" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="U12" s="18"/>
+      <c r="V12" s="18"/>
+      <c r="W12" s="18"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Fix displaying of status remarks
</commit_message>
<xml_diff>
--- a/PR Summary.xlsx
+++ b/PR Summary.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
-  <si>
-    <t>PR Summary 2021</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+  <si>
+    <t>PR Summary 2022</t>
   </si>
   <si>
     <t>PURCHASE REQUEST</t>
@@ -92,139 +92,61 @@
     <t>End User's Comments</t>
   </si>
   <si>
-    <t>2021-04-01</t>
-  </si>
-  <si>
-    <t>cons</t>
-  </si>
-  <si>
-    <t>Monitor Table and Shelves for ASPA Purpose</t>
-  </si>
-  <si>
-    <t>Monitor Table and Shelves for ASPA Enduse</t>
-  </si>
-  <si>
-    <t>ITB21-1553-CNPR</t>
-  </si>
-  <si>
-    <t>Henne</t>
+    <t>2022-03-15</t>
+  </si>
+  <si>
+    <t>CENPRI-BAGO</t>
+  </si>
+  <si>
+    <t>DRINKING WATER FOR ALL EMPLOYEES</t>
+  </si>
+  <si>
+    <t>CENPRI-EMPLOYEES</t>
+  </si>
+  <si>
+    <t>HRB22-1000-CNPR</t>
+  </si>
+  <si>
+    <t>SYNDEY SINORO</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mouse </t>
-  </si>
-  <si>
-    <t xml:space="preserve">03.03.2021 - Delivered DR# 2444-CNPR
+    <t>gal/s</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distilled Drinking Water slim with faucet gallons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03.15.2022 - Delivered DR# 1000-CNPR
+03.15.2022 - Delivered DR# 1001-CNPR
 </t>
   </si>
   <si>
     <t>Fully Delivered</t>
   </si>
   <si>
-    <t>May 10, 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyboard </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 01.01.70</t>
-  </si>
-  <si>
-    <t>Cancelled</t>
-  </si>
-  <si>
-    <t>May 11, 2021</t>
-  </si>
-  <si>
-    <t>✓</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitor </t>
-  </si>
-  <si>
-    <t>Canvassing Ongoing  
--On Hold Date: 2021-03-03 03:42:36
- -On Hold By: Jonah Benares</t>
-  </si>
-  <si>
-    <t>On-Hold</t>
-  </si>
-  <si>
-    <t>May 12, 2021</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPU </t>
-  </si>
-  <si>
-    <t>cancel 03.03.21</t>
-  </si>
-  <si>
-    <t>May 13, 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speaker </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canvassing Ongoing 
+    <t>Mar 15, 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distilled Drinking Water round neck gallons </t>
+  </si>
+  <si>
+    <t>bot/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distilled Drinking 500ml </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03.15.2022 - Delivered DR# 1000-CNPR
+03.15.2022 - Delivered DR# 1001-CNPR
+03.15.2022 - Delivered DR# 1002-CNPR
 </t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>May 14, 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- -2021-03-11
- -A &amp; M Medcare Products Distributors
- -575.00
- -3</t>
-  </si>
-  <si>
-    <t>2021-03-09</t>
-  </si>
-  <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t>IT Sample</t>
-  </si>
-  <si>
-    <t>ITB21-1556-CNPR</t>
-  </si>
-  <si>
-    <t>Jonah Benares</t>
-  </si>
-  <si>
-    <t>pc</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>2021-11-23</t>
-  </si>
-  <si>
-    <t>Mar 9, 2021</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
 </sst>
 </file>
@@ -232,7 +154,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -260,17 +182,8 @@
       <color rgb="FF000000"/>
       <name val="Arial Black"/>
     </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff0000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,18 +196,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFbcffc7"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFcacaca"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFd2deff"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -319,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="8">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -342,45 +243,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="4" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -682,10 +544,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -694,23 +556,23 @@
     <col min="2" max="2" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="25.85083" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="50.559082" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="49.416504" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="38.847656" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="19.995117" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="60.128174" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="43.560791" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="44.703369" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="23.422852" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -828,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="6">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>31</v>
@@ -858,411 +720,118 @@
       <c r="W5" s="5"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="6">
         <v>0</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="5">
         <v>2</v>
       </c>
-      <c r="K6" s="10">
-        <v>3</v>
-      </c>
-      <c r="L6" s="10" t="s">
+      <c r="K6" s="6">
+        <v>20</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="O6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="T6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="6">
         <v>0</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="5">
         <v>3</v>
       </c>
-      <c r="K7" s="15">
-        <v>1</v>
-      </c>
-      <c r="L7" s="15" t="s">
+      <c r="K7" s="6">
+        <v>100</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="S7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="T7" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="10">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9">
-        <v>4</v>
-      </c>
-      <c r="K8" s="10">
-        <v>4</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="S8" s="9" t="s">
+      <c r="M7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="T8" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="19">
-        <v>0</v>
-      </c>
-      <c r="J9" s="18">
-        <v>5</v>
-      </c>
-      <c r="K9" s="19">
-        <v>3</v>
-      </c>
-      <c r="L9" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="N9" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="S9" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="T9" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="U9" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" s="19">
-        <v>0</v>
-      </c>
-      <c r="J10" s="18">
-        <v>1</v>
-      </c>
-      <c r="K10" s="19">
-        <v>15</v>
-      </c>
-      <c r="L10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="N10" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="O10" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="P10" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q10" s="19">
-        <v>300</v>
-      </c>
-      <c r="R10" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="S10" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="T10" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="19">
-        <v>0</v>
-      </c>
-      <c r="J11" s="18">
-        <v>2</v>
-      </c>
-      <c r="K11" s="19">
-        <v>5</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="N11" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="S11" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="T11" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="19">
-        <v>0</v>
-      </c>
-      <c r="J12" s="18">
-        <v>3</v>
-      </c>
-      <c r="K12" s="19">
-        <v>10</v>
-      </c>
-      <c r="L12" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="O12" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="S12" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="T12" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>